<commit_message>
Creación 09-enero 02/02/2026 21:00
</commit_message>
<xml_diff>
--- a/2026/04-ENERO/informe_cripto.xlsx
+++ b/2026/04-ENERO/informe_cripto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1131a124248a455a/Escritorio/Oliver Preparacion Profesional/365-python-challenge/2026/04-ENERO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_293FAAE16AF65BB14EF7B9A112CB9B2B25F66D77" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F0917E5-B21D-4311-A92D-933736E33C99}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_293FAAE16AF65B21CDF02D8114CB9B2B25F66D77" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3048404-C44D-4CFC-9929-8583EB1D0DF4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -343,7 +343,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-ECC6-4B04-A782-750DDE931FDF}"/>
+              <c16:uniqueId val="{00000000-FBFA-41F9-8CA3-47CCFE35425E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -559,7 +559,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DC4F-4BF8-88E0-8298F149BD3C}"/>
+              <c16:uniqueId val="{00000000-6F0D-438B-AD9A-942A683DD775}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -759,7 +759,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4941-4197-91F1-A0A4C532FE31}"/>
+              <c16:uniqueId val="{00000000-879F-422D-A1BD-F9712E5848A5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>

</xml_diff>